<commit_message>
modified:   "tests/\347\244\272\344\276\213 - \345\257\271\346\257\224.xlsx"
</commit_message>
<xml_diff>
--- a/tests/示例 - 对比.xlsx
+++ b/tests/示例 - 对比.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="28">
   <si>
     <t>加value</t>
   </si>
@@ -48,43 +48,58 @@
     <t>第5次考试</t>
   </si>
   <si>
+    <t>第6次考试</t>
+  </si>
+  <si>
     <t>备注</t>
   </si>
   <si>
+    <t>易昭改</t>
+  </si>
+  <si>
+    <t>这里的单元格是合并的</t>
+  </si>
+  <si>
+    <t>戎保</t>
+  </si>
+  <si>
+    <t>东方艺</t>
+  </si>
+  <si>
+    <t>松邦</t>
+  </si>
+  <si>
+    <t>辛阚婷</t>
+  </si>
+  <si>
+    <t>张三</t>
+  </si>
+  <si>
+    <t>李四</t>
+  </si>
+  <si>
+    <t>芮佑康</t>
+  </si>
+  <si>
+    <t>郎国邦</t>
+  </si>
+  <si>
+    <t>王五</t>
+  </si>
+  <si>
+    <t>庾莺</t>
+  </si>
+  <si>
+    <t>顾成</t>
+  </si>
+  <si>
+    <t>这里是表尾</t>
+  </si>
+  <si>
     <t>易昭</t>
   </si>
   <si>
-    <t>这里的单元格是合并的</t>
-  </si>
-  <si>
-    <t>戎保</t>
-  </si>
-  <si>
     <t>孟姬飘</t>
-  </si>
-  <si>
-    <t>东方艺</t>
-  </si>
-  <si>
-    <t>松邦</t>
-  </si>
-  <si>
-    <t>辛阚婷</t>
-  </si>
-  <si>
-    <t>芮佑康</t>
-  </si>
-  <si>
-    <t>郎国邦</t>
-  </si>
-  <si>
-    <t>庾莺</t>
-  </si>
-  <si>
-    <t>顾成</t>
-  </si>
-  <si>
-    <t>这里是表尾</t>
   </si>
 </sst>
 </file>
@@ -92,10 +107,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -107,45 +122,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -160,22 +144,37 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -205,28 +204,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -243,12 +220,50 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="37">
     <fill>
@@ -283,102 +298,180 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -386,84 +479,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -551,15 +566,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -575,12 +581,34 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -604,32 +632,19 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -641,145 +656,145 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="11">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="10">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="8">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="8">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0">
+    <xf numFmtId="0" fontId="2" fillId="36" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="35" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0">
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -823,16 +838,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1273,10 +1288,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1284,12 +1299,12 @@
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="1" customWidth="1"/>
-    <col min="4" max="7" width="15" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="1" customWidth="1"/>
+    <col min="4" max="8" width="15" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1300,8 +1315,9 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
-    </row>
-    <row r="2" ht="25" customHeight="1" spans="1:8">
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" ht="25" customHeight="1" spans="1:9">
       <c r="A2" s="12" t="s">
         <v>3</v>
       </c>
@@ -1326,13 +1342,16 @@
       <c r="H2" s="12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" ht="25" customHeight="1" spans="1:8">
+      <c r="I2" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" ht="25" customHeight="1" spans="1:9">
       <c r="A3" s="13">
         <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="13">
         <v>75</v>
@@ -1349,22 +1368,25 @@
       <c r="G3" s="13">
         <v>82</v>
       </c>
-      <c r="H3" s="15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" ht="25" customHeight="1" spans="1:8">
+      <c r="H3" s="13">
+        <v>83</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" ht="25" customHeight="1" spans="1:9">
       <c r="A4" s="13">
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="13">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="D4" s="13">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="E4" s="13">
         <v>75</v>
@@ -1375,227 +1397,303 @@
       <c r="G4" s="13">
         <v>95</v>
       </c>
-      <c r="H4" s="16"/>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:8">
+      <c r="H4" s="13">
+        <v>85</v>
+      </c>
+      <c r="I4" s="18"/>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:9">
       <c r="A5" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="13">
+        <v>85</v>
+      </c>
+      <c r="D5" s="13">
+        <v>82</v>
+      </c>
+      <c r="E5" s="13">
+        <v>83</v>
+      </c>
+      <c r="F5" s="13">
         <v>90</v>
       </c>
-      <c r="D5" s="13">
-        <v>88</v>
-      </c>
-      <c r="E5" s="13">
-        <v>78</v>
-      </c>
-      <c r="F5" s="13">
-        <v>65</v>
-      </c>
       <c r="G5" s="13">
-        <v>62</v>
-      </c>
-      <c r="H5" s="16"/>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:8">
+        <v>84</v>
+      </c>
+      <c r="H5" s="13">
+        <v>82</v>
+      </c>
+      <c r="I5" s="18"/>
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:9">
       <c r="A6" s="13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" s="13">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="D6" s="13">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E6" s="13">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F6" s="13">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="G6" s="13">
+        <v>76</v>
+      </c>
+      <c r="H6" s="13">
+        <v>80</v>
+      </c>
+      <c r="I6" s="18"/>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:9">
+      <c r="A7" s="13">
+        <v>6</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="13">
         <v>84</v>
-      </c>
-      <c r="H6" s="16"/>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:8">
-      <c r="A7" s="13">
-        <v>5</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="13">
-        <v>72</v>
       </c>
       <c r="D7" s="13">
         <v>75</v>
       </c>
       <c r="E7" s="13">
+        <v>76</v>
+      </c>
+      <c r="F7" s="13">
+        <v>82</v>
+      </c>
+      <c r="G7" s="13">
+        <v>65</v>
+      </c>
+      <c r="H7" s="13">
+        <v>88</v>
+      </c>
+      <c r="I7" s="18"/>
+    </row>
+    <row r="8" ht="25" customHeight="1" spans="1:9">
+      <c r="A8" s="13"/>
+      <c r="B8" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="13">
+        <v>72</v>
+      </c>
+      <c r="D8" s="13">
+        <v>65</v>
+      </c>
+      <c r="E8" s="13">
+        <v>82</v>
+      </c>
+      <c r="F8" s="13">
+        <v>98</v>
+      </c>
+      <c r="G8" s="13">
+        <v>77</v>
+      </c>
+      <c r="H8" s="13">
+        <v>79</v>
+      </c>
+      <c r="I8" s="18"/>
+    </row>
+    <row r="9" ht="25" customHeight="1" spans="1:9">
+      <c r="A9" s="13"/>
+      <c r="B9" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="13">
+        <v>85</v>
+      </c>
+      <c r="D9" s="13">
+        <v>76</v>
+      </c>
+      <c r="E9" s="13">
         <v>84</v>
       </c>
-      <c r="F7" s="13">
-        <v>73</v>
-      </c>
-      <c r="G7" s="13">
+      <c r="F9" s="13">
+        <v>78</v>
+      </c>
+      <c r="G9" s="13">
+        <v>86</v>
+      </c>
+      <c r="H9" s="13">
+        <v>86</v>
+      </c>
+      <c r="I9" s="18"/>
+    </row>
+    <row r="10" ht="25" customHeight="1" spans="1:9">
+      <c r="A10" s="13">
+        <v>7</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="13">
+        <v>72</v>
+      </c>
+      <c r="D10" s="13">
+        <v>78</v>
+      </c>
+      <c r="E10" s="13">
+        <v>82</v>
+      </c>
+      <c r="F10" s="13">
+        <v>88</v>
+      </c>
+      <c r="G10" s="13">
+        <v>89</v>
+      </c>
+      <c r="H10" s="13">
+        <v>90</v>
+      </c>
+      <c r="I10" s="18"/>
+    </row>
+    <row r="11" ht="25" customHeight="1" spans="1:9">
+      <c r="A11" s="13">
+        <v>8</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="13">
+        <v>63</v>
+      </c>
+      <c r="D11" s="13">
+        <v>74</v>
+      </c>
+      <c r="E11" s="13">
+        <v>85</v>
+      </c>
+      <c r="F11" s="13">
+        <v>96</v>
+      </c>
+      <c r="G11" s="13">
+        <v>98</v>
+      </c>
+      <c r="H11" s="13">
         <v>76</v>
       </c>
-      <c r="H7" s="16"/>
-    </row>
-    <row r="8" ht="25" customHeight="1" spans="1:8">
-      <c r="A8" s="13">
-        <v>6</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="13">
-        <v>48</v>
-      </c>
-      <c r="D8" s="13">
-        <v>75</v>
-      </c>
-      <c r="E8" s="13">
-        <v>36</v>
-      </c>
-      <c r="F8" s="13">
-        <v>82</v>
-      </c>
-      <c r="G8" s="13">
+      <c r="I11" s="18"/>
+    </row>
+    <row r="12" ht="25" customHeight="1" spans="1:9">
+      <c r="A12" s="13"/>
+      <c r="B12" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="13">
+        <v>85</v>
+      </c>
+      <c r="D12" s="13">
+        <v>86</v>
+      </c>
+      <c r="E12" s="13">
+        <v>79</v>
+      </c>
+      <c r="F12" s="13">
+        <v>91</v>
+      </c>
+      <c r="G12" s="13">
+        <v>88</v>
+      </c>
+      <c r="H12" s="13">
+        <v>83</v>
+      </c>
+      <c r="I12" s="18"/>
+    </row>
+    <row r="13" ht="25" customHeight="1" spans="1:9">
+      <c r="A13" s="13">
+        <v>9</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="13">
+        <v>78</v>
+      </c>
+      <c r="D13" s="13">
+        <v>98</v>
+      </c>
+      <c r="E13" s="13">
+        <v>62</v>
+      </c>
+      <c r="F13" s="13">
+        <v>85</v>
+      </c>
+      <c r="G13" s="13">
+        <v>72</v>
+      </c>
+      <c r="H13" s="13">
+        <v>72</v>
+      </c>
+      <c r="I13" s="18"/>
+    </row>
+    <row r="14" ht="25" customHeight="1" spans="1:9">
+      <c r="A14" s="13">
+        <v>10</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="13">
         <v>65</v>
       </c>
-      <c r="H8" s="16"/>
-    </row>
-    <row r="9" ht="25" customHeight="1" spans="1:8">
-      <c r="A9" s="13">
-        <v>7</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="13">
-        <v>72</v>
-      </c>
-      <c r="D9" s="13">
-        <v>78</v>
-      </c>
-      <c r="E9" s="13">
-        <v>82</v>
-      </c>
-      <c r="F9" s="13">
+      <c r="D14" s="13">
+        <v>84</v>
+      </c>
+      <c r="E14" s="13">
+        <v>85</v>
+      </c>
+      <c r="F14" s="13">
         <v>88</v>
       </c>
-      <c r="G9" s="13">
-        <v>89</v>
-      </c>
-      <c r="H9" s="16"/>
-    </row>
-    <row r="10" ht="25" customHeight="1" spans="1:8">
-      <c r="A10" s="13">
-        <v>8</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="13">
-        <v>63</v>
-      </c>
-      <c r="D10" s="13">
-        <v>74</v>
-      </c>
-      <c r="E10" s="13">
-        <v>85</v>
-      </c>
-      <c r="F10" s="13">
-        <v>96</v>
-      </c>
-      <c r="G10" s="13">
-        <v>98</v>
-      </c>
-      <c r="H10" s="16"/>
-    </row>
-    <row r="11" ht="25" customHeight="1" spans="1:8">
-      <c r="A11" s="13">
-        <v>9</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="13">
-        <v>53</v>
-      </c>
-      <c r="D11" s="13">
-        <v>64</v>
-      </c>
-      <c r="E11" s="13">
-        <v>62</v>
-      </c>
-      <c r="F11" s="13">
-        <v>85</v>
-      </c>
-      <c r="G11" s="13">
-        <v>72</v>
-      </c>
-      <c r="H11" s="16"/>
-    </row>
-    <row r="12" ht="25" customHeight="1" spans="1:8">
-      <c r="A12" s="13">
-        <v>10</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="13">
-        <v>65</v>
-      </c>
-      <c r="D12" s="13">
-        <v>84</v>
-      </c>
-      <c r="E12" s="13">
-        <v>85</v>
-      </c>
-      <c r="F12" s="13">
-        <v>88</v>
-      </c>
-      <c r="G12" s="13">
+      <c r="G14" s="13">
         <v>95</v>
       </c>
-      <c r="H12" s="16"/>
-    </row>
-    <row r="13" ht="25" customHeight="1" spans="1:8">
-      <c r="A13" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-    </row>
-    <row r="21" spans="12:14">
-      <c r="L21"/>
-      <c r="M21"/>
-      <c r="N21"/>
-    </row>
-    <row r="22" spans="12:14">
-      <c r="L22"/>
-      <c r="M22"/>
-      <c r="N22"/>
+      <c r="H14" s="13">
+        <v>95</v>
+      </c>
+      <c r="I14" s="18"/>
+    </row>
+    <row r="15" ht="25" customHeight="1" spans="1:9">
+      <c r="A15" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+    </row>
+    <row r="23" spans="13:15">
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+    </row>
+    <row r="24" spans="13:15">
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="H3:H12"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="I3:I14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1656,7 +1754,7 @@
         <v>9</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" ht="25" customHeight="1" spans="1:8">
@@ -1664,7 +1762,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C3" s="5">
         <v>75</v>
@@ -1682,7 +1780,7 @@
         <v>82</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:8">
@@ -1690,7 +1788,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="5">
         <v>58</v>
@@ -1714,7 +1812,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C5" s="5">
         <v>90</v>
@@ -1810,7 +1908,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C9" s="5">
         <v>72</v>
@@ -1834,7 +1932,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C10" s="5">
         <v>63</v>
@@ -1858,7 +1956,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C11" s="5">
         <v>53</v>
@@ -1882,7 +1980,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C12" s="5">
         <v>65</v>
@@ -1903,7 +2001,7 @@
     </row>
     <row r="13" ht="25" customHeight="1" spans="1:8">
       <c r="A13" s="10" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>

</xml_diff>

<commit_message>
modified:   excel_operate/list_operate.py 	modified:   excel_operate/sheet_comparison.py 	modified:   "tests/\347\244\272\344\276\213 - \345\257\271\346\257\224.xlsx" 	modified:   "tests/\347\244\272\344\276\213.xlsx"
</commit_message>
<xml_diff>
--- a/tests/示例 - 对比.xlsx
+++ b/tests/示例 - 对比.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="28">
   <si>
     <t>加value</t>
   </si>
@@ -36,64 +36,64 @@
     <t>第1次考试</t>
   </si>
   <si>
+    <t>第3次考试</t>
+  </si>
+  <si>
+    <t>第4次考试</t>
+  </si>
+  <si>
+    <t>第5次考试</t>
+  </si>
+  <si>
+    <t>第6次考试</t>
+  </si>
+  <si>
+    <t>备注</t>
+  </si>
+  <si>
+    <t>易昭改</t>
+  </si>
+  <si>
+    <t>这里的单元格是合并的</t>
+  </si>
+  <si>
+    <t>戎保</t>
+  </si>
+  <si>
+    <t>东方艺</t>
+  </si>
+  <si>
+    <t>松邦</t>
+  </si>
+  <si>
+    <t>辛阚婷</t>
+  </si>
+  <si>
+    <t>张三</t>
+  </si>
+  <si>
+    <t>李四</t>
+  </si>
+  <si>
+    <t>芮佑康</t>
+  </si>
+  <si>
+    <t>郎国邦</t>
+  </si>
+  <si>
+    <t>王五</t>
+  </si>
+  <si>
+    <t>庾莺</t>
+  </si>
+  <si>
+    <t>顾成</t>
+  </si>
+  <si>
+    <t>这里是表尾</t>
+  </si>
+  <si>
     <t>第2次考试</t>
-  </si>
-  <si>
-    <t>第3次考试</t>
-  </si>
-  <si>
-    <t>第4次考试</t>
-  </si>
-  <si>
-    <t>第5次考试</t>
-  </si>
-  <si>
-    <t>第6次考试</t>
-  </si>
-  <si>
-    <t>备注</t>
-  </si>
-  <si>
-    <t>易昭改</t>
-  </si>
-  <si>
-    <t>这里的单元格是合并的</t>
-  </si>
-  <si>
-    <t>戎保</t>
-  </si>
-  <si>
-    <t>东方艺</t>
-  </si>
-  <si>
-    <t>松邦</t>
-  </si>
-  <si>
-    <t>辛阚婷</t>
-  </si>
-  <si>
-    <t>张三</t>
-  </si>
-  <si>
-    <t>李四</t>
-  </si>
-  <si>
-    <t>芮佑康</t>
-  </si>
-  <si>
-    <t>郎国邦</t>
-  </si>
-  <si>
-    <t>王五</t>
-  </si>
-  <si>
-    <t>庾莺</t>
-  </si>
-  <si>
-    <t>顾成</t>
-  </si>
-  <si>
-    <t>这里是表尾</t>
   </si>
   <si>
     <t>易昭</t>
@@ -108,8 +108,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -122,14 +122,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -142,9 +143,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -159,17 +159,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -180,11 +172,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -228,8 +219,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -251,7 +251,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -259,7 +259,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -298,187 +298,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -552,36 +552,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -601,6 +571,30 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -629,11 +623,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -656,10 +656,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="6">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="8">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0">
@@ -668,133 +668,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="11">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="11">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="8">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="8">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="7">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -838,16 +838,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1288,23 +1288,24 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D2" sqref="D$1:D$1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="1" customWidth="1"/>
-    <col min="4" max="8" width="15" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="1" customWidth="1"/>
+    <col min="4" max="7" width="15" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8" style="1" customWidth="1"/>
+    <col min="9" max="16373" width="9" style="1" customWidth="1"/>
+    <col min="16374" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1315,9 +1316,8 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" ht="25" customHeight="1" spans="1:9">
+    </row>
+    <row r="2" ht="25" customHeight="1" spans="1:8">
       <c r="A2" s="12" t="s">
         <v>3</v>
       </c>
@@ -1342,358 +1342,308 @@
       <c r="H2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" ht="25" customHeight="1" spans="1:9">
+    </row>
+    <row r="3" ht="25" customHeight="1" spans="1:8">
       <c r="A3" s="13">
         <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="13">
         <v>75</v>
       </c>
       <c r="D3" s="13">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E3" s="13">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="F3" s="13">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G3" s="13">
-        <v>82</v>
-      </c>
-      <c r="H3" s="13">
         <v>83</v>
       </c>
-      <c r="I3" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" ht="25" customHeight="1" spans="1:9">
+      <c r="H3" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" ht="25" customHeight="1" spans="1:8">
       <c r="A4" s="13">
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="13">
         <v>85</v>
       </c>
       <c r="D4" s="13">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="E4" s="13">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="F4" s="13">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="G4" s="13">
-        <v>95</v>
-      </c>
-      <c r="H4" s="13">
         <v>85</v>
       </c>
-      <c r="I4" s="18"/>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:9">
+      <c r="H4" s="16"/>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:8">
       <c r="A5" s="13">
         <v>4</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="13">
         <v>85</v>
       </c>
       <c r="D5" s="13">
+        <v>83</v>
+      </c>
+      <c r="E5" s="13">
+        <v>90</v>
+      </c>
+      <c r="F5" s="13">
+        <v>84</v>
+      </c>
+      <c r="G5" s="13">
         <v>82</v>
       </c>
-      <c r="E5" s="13">
-        <v>83</v>
-      </c>
-      <c r="F5" s="13">
-        <v>90</v>
-      </c>
-      <c r="G5" s="13">
-        <v>84</v>
-      </c>
-      <c r="H5" s="13">
-        <v>82</v>
-      </c>
-      <c r="I5" s="18"/>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:9">
+      <c r="H5" s="16"/>
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:8">
       <c r="A6" s="13">
         <v>5</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="13">
         <v>72</v>
       </c>
       <c r="D6" s="13">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="E6" s="13">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="F6" s="13">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G6" s="13">
-        <v>76</v>
-      </c>
-      <c r="H6" s="13">
         <v>80</v>
       </c>
-      <c r="I6" s="18"/>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:9">
+      <c r="H6" s="16"/>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:8">
       <c r="A7" s="13">
         <v>6</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="13">
         <v>84</v>
       </c>
       <c r="D7" s="13">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E7" s="13">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="F7" s="13">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="G7" s="13">
-        <v>65</v>
-      </c>
-      <c r="H7" s="13">
         <v>88</v>
       </c>
-      <c r="I7" s="18"/>
-    </row>
-    <row r="8" ht="25" customHeight="1" spans="1:9">
+      <c r="H7" s="16"/>
+    </row>
+    <row r="8" ht="25" customHeight="1" spans="1:8">
       <c r="A8" s="13"/>
       <c r="B8" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="13">
         <v>72</v>
       </c>
       <c r="D8" s="13">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="E8" s="13">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="F8" s="13">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="G8" s="13">
-        <v>77</v>
-      </c>
-      <c r="H8" s="13">
         <v>79</v>
       </c>
-      <c r="I8" s="18"/>
-    </row>
-    <row r="9" ht="25" customHeight="1" spans="1:9">
+      <c r="H8" s="16"/>
+    </row>
+    <row r="9" ht="25" customHeight="1" spans="1:8">
       <c r="A9" s="13"/>
       <c r="B9" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="13">
         <v>85</v>
       </c>
       <c r="D9" s="13">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="E9" s="13">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="F9" s="13">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="G9" s="13">
         <v>86</v>
       </c>
-      <c r="H9" s="13">
-        <v>86</v>
-      </c>
-      <c r="I9" s="18"/>
-    </row>
-    <row r="10" ht="25" customHeight="1" spans="1:9">
+      <c r="H9" s="16"/>
+    </row>
+    <row r="10" ht="25" customHeight="1" spans="1:8">
       <c r="A10" s="13">
         <v>7</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="13">
         <v>72</v>
       </c>
       <c r="D10" s="13">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E10" s="13">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="F10" s="13">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G10" s="13">
-        <v>89</v>
-      </c>
-      <c r="H10" s="13">
         <v>90</v>
       </c>
-      <c r="I10" s="18"/>
-    </row>
-    <row r="11" ht="25" customHeight="1" spans="1:9">
+      <c r="H10" s="16"/>
+    </row>
+    <row r="11" ht="25" customHeight="1" spans="1:8">
       <c r="A11" s="13">
         <v>8</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="13">
         <v>63</v>
       </c>
       <c r="D11" s="13">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="E11" s="13">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="F11" s="13">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G11" s="13">
-        <v>98</v>
-      </c>
-      <c r="H11" s="13">
         <v>76</v>
       </c>
-      <c r="I11" s="18"/>
-    </row>
-    <row r="12" ht="25" customHeight="1" spans="1:9">
+      <c r="H11" s="16"/>
+    </row>
+    <row r="12" ht="25" customHeight="1" spans="1:8">
       <c r="A12" s="13"/>
       <c r="B12" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="13">
         <v>85</v>
       </c>
       <c r="D12" s="13">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E12" s="13">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="F12" s="13">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G12" s="13">
-        <v>88</v>
-      </c>
-      <c r="H12" s="13">
         <v>83</v>
       </c>
-      <c r="I12" s="18"/>
-    </row>
-    <row r="13" ht="25" customHeight="1" spans="1:9">
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" ht="25" customHeight="1" spans="1:8">
       <c r="A13" s="13">
         <v>9</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="13">
         <v>78</v>
       </c>
       <c r="D13" s="13">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="E13" s="13">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="F13" s="13">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="G13" s="13">
         <v>72</v>
       </c>
-      <c r="H13" s="13">
-        <v>72</v>
-      </c>
-      <c r="I13" s="18"/>
-    </row>
-    <row r="14" ht="25" customHeight="1" spans="1:9">
+      <c r="H13" s="16"/>
+    </row>
+    <row r="14" ht="25" customHeight="1" spans="1:8">
       <c r="A14" s="13">
         <v>10</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="13">
         <v>65</v>
       </c>
       <c r="D14" s="13">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E14" s="13">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F14" s="13">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="G14" s="13">
         <v>95</v>
       </c>
-      <c r="H14" s="13">
-        <v>95</v>
-      </c>
-      <c r="I14" s="18"/>
-    </row>
-    <row r="15" ht="25" customHeight="1" spans="1:9">
-      <c r="A15" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-    </row>
-    <row r="23" spans="13:15">
-      <c r="M23"/>
-      <c r="N23"/>
-      <c r="O23"/>
-    </row>
-    <row r="24" spans="13:15">
-      <c r="M24"/>
-      <c r="N24"/>
-      <c r="O24"/>
+      <c r="H14" s="16"/>
+    </row>
+    <row r="15" ht="25" customHeight="1" spans="1:8">
+      <c r="A15" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="I3:I14"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="H3:H14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1742,19 +1692,19 @@
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="H2" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" ht="25" customHeight="1" spans="1:8">
@@ -1780,7 +1730,7 @@
         <v>82</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:8">
@@ -1788,7 +1738,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="5">
         <v>58</v>
@@ -1836,7 +1786,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="5">
         <v>85</v>
@@ -1860,7 +1810,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="5">
         <v>72</v>
@@ -1884,7 +1834,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="5">
         <v>48</v>
@@ -1908,7 +1858,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="5">
         <v>72</v>
@@ -1932,7 +1882,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="5">
         <v>63</v>
@@ -1956,7 +1906,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="5">
         <v>53</v>
@@ -1980,7 +1930,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="5">
         <v>65</v>
@@ -2001,7 +1951,7 @@
     </row>
     <row r="13" ht="25" customHeight="1" spans="1:8">
       <c r="A13" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>

</xml_diff>